<commit_message>
Reorganize result files and add new datasets (xlsx)
Move legacy Shopee result XLSX files into result/lama/, add Tokopedia result files to result/lama/, and update several Tokopedia result/preprocessed XLSX files. Also add dataset/nyoba_preprocessed.xlsx and modify dataset/new_dataset_program.xlsx. These changes tidy up result/ by archiving older Shopee files and introduce new Tokopedia and preprocessed dataset artifacts (binary XLSX files).
</commit_message>
<xml_diff>
--- a/result/crawling_from_tokopedia.xlsx
+++ b/result/crawling_from_tokopedia.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,12 +453,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>D***a</t>
+          <t>Taufik</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>cukup untuk yang mau game pakai sens rendah halus licin TPI kontrolnya masih dapat tebel</t>
+          <t>Selalu beli laptop di NVIDIA GEFORCE LAPTOP selalu aman dan laptop sampe tujuan tanpa lecet .</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -466,12 +466,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>a***n</t>
+          <t>J***s</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ukuran pas, material yg cakep dan seperti mousepad pada umumnya dengan harga yang terjangkau bisa dibilang.</t>
+          <t>Pelayanan terbaik. Banyak bonusnya ternyata. Terima kasih 🙏</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -479,12 +479,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Aripin</t>
+          <t>N***l</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BARANG : Sesuai ekspektasi SELLER : Responsif COURIER : Tidak ada masalah</t>
+          <t>Barang sampai dengan packing aman dan mulus sudah di cek dan tes devicenya berjalan normal semoga awet dan tinggal aktifkan office 2021 home student</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -492,12 +492,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>D***e</t>
+          <t>D***o</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>sat set, psen kmren bsknya lgsg smpe dpn rumah. hasil gambar bagus, tidak tipis, anti slip jg ckup tebal jd ga suka geser, looks dan kualitas ckp oke. cmn di bbrp jaitan ada warna kaya luntur (koreksi klo salah) yg sy khawatir klo kringetan bkal ngrusak wrnanya. satu lg, isi paket saya ada smpah</t>
+          <t>pelayanan cepat, pengiriman tepat waktu, semoga awet, terima kasih bonusnya</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -505,275 +505,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>d****</t>
+          <t>p***z</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mantep lah, ketebalan ok, ukuran sesuai, motif jernih,kalau buat peforma kayaknya sih ok (belum coba buat game)</t>
+          <t>bad service jadi malas pengen beli produk lainnya dari toko ini, ga bisa dibatalin padahal mau beli laptop yg lebih bagus gara gara katanya udh dikirim padahal resi cetak baru lusa sorenya hadeuh kurang akurat sekali informasinya jadi jangan mudah beli di toko ini. not recommended, mana barang bermasalah lagi kemasan cuma pake bubble tipis hadeuh gmn sih ini yg bener aja kecewa berat spek kaleng dijual harga langit</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Abie</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Barang ok, bagus. Pengiriman cepat, recommended.</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>F***e</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Kualitas pengerjaan: BAGUS Bahan: BAGUS Perakitan: Bagus Barang sampai tapi yg sampai nya warna hitam bukan yg putih 🤦‍♂️</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>M***h</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Mousepad nya sangat nyaman dipakai, bahannya halus dan cetakannya tajam. Mantap banget.. Makasih kak</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>I***a</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Bahan dan barang nya bagus sebenarnya, tapi karena pengiriman agak lama, jadi kayak ada bekas lekukannya, dan ya jujur jujuran aja ya seperti di video packingnya cuman kardus, tapi dari kualitas barang nya bagus kok minusnya cuman itu aja</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>T***h</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Kualitas bagus buat harganya, motif juga bagus. tebel juga enak buat setup</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>irsyad</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>bagus banget plisss, bahannya ga keset (licin) dan tebel jahitannya juga rapih dan warnnya juga real sama kaya di foto produk, worth it !</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>R***w</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Bahan: Bagus responsif dan tidak cacat jahitan😍 Alhamdulillah barang sampai dengan selamat dan bagus. Minusnya disaya aja masih nabung buat rakit PC, bantu do'ain ya min supaya cepat kebeli PC nya 😇🤗</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>T***c</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Quality of work: BAGUS Material: Enak buat mouse</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Ida</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>ukuran sesuai, bahan dan material baik, cukup halus.. mouse meluncur dengan lancar diatasnya..</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Rey</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Proses cepat, bahan bagus, gak licin, sesuai harga, mantap</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>R***p</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Bahan berbau tajam (jadi pertimbangan), jahitan masih kurang rapi, selain itu motif, desain dan lainnya bagus... Sesuai harga</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>L***u</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Bahan adem, tebel, bagus gk licin dan gk terlalu keset juga, oke buat mousenya. Minus nya bahan bawah nya kurang keset, jadi suka geser deskmat nya. Minus juga pinggirannya melengkung, karena emg paketnya digulung, jdi pinggirannya susah buat lurus lagi, butuh waktu. Overall oke. Murah juga sih.</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Samet</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Kualitas Dari Mousepad sangat bagus Dan tebal. gambarnya rapi Dan jelas. Sangat recommend</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>N***p</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>overall dari bahan oke dan bagus, designnya juga keren tapi yang saya kecewain adalah saat saya teliti ada noda biru disekitar warna putih. itu saja keluhan saya.</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>K***y</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Bahan: Halus dan Tebal Barangnya bagus, halus, dan licin buat mouse, mantap deh.</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>R***a</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Kualitas nya mantap dan permukaan nya halus licin, serta anti slip</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Alice</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Lumayan nih gaes pas kena flash sale ga sampe 50rb. bahan lumayan baik, cukup rapih, tapi ya jangan bandingkan dengan yg diatas serratus ribuan ya, tapi ini bagus lah. proses cepat langsung dikitim, kurir juga sat set. lumayan buat ganti suasana setup. trimakasih ya</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Ardie</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>paketnya aman banget,mousepadnya bagus banget padahal murah walaupun ada miss paint dikit gpp soalnya harganya murah banget terus bahan mousepadnya tebelll</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>X***f</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Bahannya bagus, kayaknya ini lebih ke tipe speed (agak licin). Jahitan pinggirannya juga rapi. Kualitas gambarnya bagus (tidak blur), tapi warna gambarnya agak wash out (kurang pekat warnanya). Ntah ini memang warna asli designnya seperti ini atau ngga. Untuk deskmat harga under 100k udah oke 👍</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>P***r</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>bahannya lumayan buat harga segitu , juga ada sedikit luntur atau noda biru kecil😁🤏🏻</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>